<commit_message>
Made if more efficient by querying just needed stuff
</commit_message>
<xml_diff>
--- a/static/excel/data.xlsx
+++ b/static/excel/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="231">
   <si>
     <t>stu_id</t>
   </si>
@@ -679,79 +679,34 @@
     <t>Science</t>
   </si>
   <si>
-    <t>New user</t>
+    <t>Sparsh Venkappa Rao</t>
   </si>
   <si>
     <t>Male</t>
   </si>
   <si>
+    <t>+917619391823</t>
+  </si>
+  <si>
     <t>MSc</t>
   </si>
   <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>new guy</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>Sparsh Venkappa Rao</t>
-  </si>
-  <si>
-    <t>+917619391823</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>xavier</t>
-  </si>
-  <si>
-    <t>PhD</t>
-  </si>
-  <si>
-    <t>12345678</t>
-  </si>
-  <si>
-    <t>mba check</t>
+    <t>Holaaaaaa</t>
   </si>
   <si>
     <t>MBA</t>
   </si>
   <si>
-    <t>555</t>
+    <t>777</t>
+  </si>
+  <si>
+    <t>New user added</t>
+  </si>
+  <si>
+    <t>23534</t>
   </si>
   <si>
     <t>666</t>
-  </si>
-  <si>
-    <t>777</t>
-  </si>
-  <si>
-    <t>999</t>
-  </si>
-  <si>
-    <t>650</t>
-  </si>
-  <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>076 1939 1823</t>
-  </si>
-  <si>
-    <t>sparshrao1@gmail.com</t>
-  </si>
-  <si>
-    <t>1234567890</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1038,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:GH15"/>
+  <dimension ref="A1:GH6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1830,7 +1785,7 @@
     </row>
     <row r="3" spans="1:190">
       <c r="A3">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
         <v>221</v>
@@ -1841,6 +1796,9 @@
       <c r="E3" t="s">
         <v>193</v>
       </c>
+      <c r="G3" t="s">
+        <v>223</v>
+      </c>
       <c r="M3" t="s">
         <v>194</v>
       </c>
@@ -1863,7 +1821,7 @@
         <v>197</v>
       </c>
       <c r="AP3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AQ3" t="s">
         <v>204</v>
@@ -1902,7 +1860,7 @@
         <v>197</v>
       </c>
       <c r="BG3" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="BH3" t="s">
         <v>197</v>
@@ -2009,7 +1967,7 @@
     </row>
     <row r="4" spans="1:190">
       <c r="A4">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>225</v>
@@ -2042,7 +2000,7 @@
         <v>197</v>
       </c>
       <c r="AP4" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="AQ4" t="s">
         <v>204</v>
@@ -2081,7 +2039,7 @@
         <v>197</v>
       </c>
       <c r="BG4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="BH4" t="s">
         <v>197</v>
@@ -2157,23 +2115,47 @@
       </c>
       <c r="DS4" t="s">
         <v>220</v>
+      </c>
+      <c r="EX4" t="s">
+        <v>213</v>
+      </c>
+      <c r="EY4" t="s">
+        <v>214</v>
+      </c>
+      <c r="EZ4" t="s">
+        <v>215</v>
+      </c>
+      <c r="FB4" t="s">
+        <v>219</v>
+      </c>
+      <c r="FD4" t="s">
+        <v>198</v>
+      </c>
+      <c r="FE4" t="s">
+        <v>199</v>
+      </c>
+      <c r="FI4" t="s">
+        <v>216</v>
+      </c>
+      <c r="FM4" t="s">
+        <v>217</v>
+      </c>
+      <c r="FN4" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:190">
       <c r="A5">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D5" t="s">
         <v>222</v>
       </c>
       <c r="E5" t="s">
         <v>193</v>
-      </c>
-      <c r="G5" t="s">
-        <v>228</v>
       </c>
       <c r="M5" t="s">
         <v>194</v>
@@ -2316,10 +2298,10 @@
     </row>
     <row r="6" spans="1:190">
       <c r="A6">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D6" t="s">
         <v>222</v>
@@ -2328,7 +2310,7 @@
         <v>193</v>
       </c>
       <c r="G6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M6" t="s">
         <v>194</v>
@@ -2391,7 +2373,7 @@
         <v>197</v>
       </c>
       <c r="BG6" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="BH6" t="s">
         <v>197</v>
@@ -2466,1557 +2448,6 @@
         <v>216</v>
       </c>
       <c r="DS6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="7" spans="1:190">
-      <c r="A7">
-        <v>64</v>
-      </c>
-      <c r="B7" t="s">
-        <v>230</v>
-      </c>
-      <c r="D7" t="s">
-        <v>222</v>
-      </c>
-      <c r="E7" t="s">
-        <v>193</v>
-      </c>
-      <c r="M7" t="s">
-        <v>194</v>
-      </c>
-      <c r="O7" t="s">
-        <v>195</v>
-      </c>
-      <c r="P7" t="s">
-        <v>196</v>
-      </c>
-      <c r="R7" t="s">
-        <v>197</v>
-      </c>
-      <c r="S7" t="s">
-        <v>198</v>
-      </c>
-      <c r="T7" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>197</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>231</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>204</v>
-      </c>
-      <c r="AR7" t="s">
-        <v>205</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV7" t="s">
-        <v>206</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>197</v>
-      </c>
-      <c r="AX7" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY7" t="s">
-        <v>208</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>208</v>
-      </c>
-      <c r="BB7" t="s">
-        <v>210</v>
-      </c>
-      <c r="BC7" t="s">
-        <v>210</v>
-      </c>
-      <c r="BD7" t="s">
-        <v>197</v>
-      </c>
-      <c r="BG7" t="s">
-        <v>232</v>
-      </c>
-      <c r="BH7" t="s">
-        <v>197</v>
-      </c>
-      <c r="BI7" t="s">
-        <v>205</v>
-      </c>
-      <c r="BM7" t="s">
-        <v>197</v>
-      </c>
-      <c r="BT7" t="s">
-        <v>198</v>
-      </c>
-      <c r="BU7" t="s">
-        <v>199</v>
-      </c>
-      <c r="BZ7" t="s">
-        <v>212</v>
-      </c>
-      <c r="CC7" t="s">
-        <v>198</v>
-      </c>
-      <c r="CD7" t="s">
-        <v>199</v>
-      </c>
-      <c r="CJ7" t="s">
-        <v>213</v>
-      </c>
-      <c r="CK7" t="s">
-        <v>214</v>
-      </c>
-      <c r="CL7" t="s">
-        <v>215</v>
-      </c>
-      <c r="CP7" t="s">
-        <v>198</v>
-      </c>
-      <c r="CQ7" t="s">
-        <v>199</v>
-      </c>
-      <c r="CU7" t="s">
-        <v>216</v>
-      </c>
-      <c r="CY7" t="s">
-        <v>217</v>
-      </c>
-      <c r="CZ7" t="s">
-        <v>217</v>
-      </c>
-      <c r="DB7" t="s">
-        <v>218</v>
-      </c>
-      <c r="DD7" t="s">
-        <v>213</v>
-      </c>
-      <c r="DE7" t="s">
-        <v>214</v>
-      </c>
-      <c r="DF7" t="s">
-        <v>215</v>
-      </c>
-      <c r="DH7" t="s">
-        <v>219</v>
-      </c>
-      <c r="DJ7" t="s">
-        <v>198</v>
-      </c>
-      <c r="DK7" t="s">
-        <v>199</v>
-      </c>
-      <c r="DO7" t="s">
-        <v>216</v>
-      </c>
-      <c r="DS7" t="s">
-        <v>220</v>
-      </c>
-      <c r="EX7" t="s">
-        <v>213</v>
-      </c>
-      <c r="EY7" t="s">
-        <v>214</v>
-      </c>
-      <c r="EZ7" t="s">
-        <v>215</v>
-      </c>
-      <c r="FB7" t="s">
-        <v>219</v>
-      </c>
-      <c r="FD7" t="s">
-        <v>198</v>
-      </c>
-      <c r="FE7" t="s">
-        <v>199</v>
-      </c>
-      <c r="FI7" t="s">
-        <v>216</v>
-      </c>
-      <c r="FM7" t="s">
-        <v>217</v>
-      </c>
-      <c r="FN7" t="s">
-        <v>217</v>
-      </c>
-      <c r="FQ7" t="s">
-        <v>213</v>
-      </c>
-      <c r="FR7" t="s">
-        <v>214</v>
-      </c>
-      <c r="FS7" t="s">
-        <v>215</v>
-      </c>
-      <c r="FU7" t="s">
-        <v>219</v>
-      </c>
-      <c r="FW7" t="s">
-        <v>198</v>
-      </c>
-      <c r="FX7" t="s">
-        <v>199</v>
-      </c>
-      <c r="GB7" t="s">
-        <v>216</v>
-      </c>
-      <c r="GF7" t="s">
-        <v>217</v>
-      </c>
-      <c r="GG7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:190">
-      <c r="A8">
-        <v>66</v>
-      </c>
-      <c r="B8" t="s">
-        <v>233</v>
-      </c>
-      <c r="D8" t="s">
-        <v>222</v>
-      </c>
-      <c r="E8" t="s">
-        <v>193</v>
-      </c>
-      <c r="M8" t="s">
-        <v>194</v>
-      </c>
-      <c r="O8" t="s">
-        <v>195</v>
-      </c>
-      <c r="P8" t="s">
-        <v>196</v>
-      </c>
-      <c r="R8" t="s">
-        <v>197</v>
-      </c>
-      <c r="S8" t="s">
-        <v>198</v>
-      </c>
-      <c r="T8" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>197</v>
-      </c>
-      <c r="AP8" t="s">
-        <v>234</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>204</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>205</v>
-      </c>
-      <c r="AS8" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV8" t="s">
-        <v>206</v>
-      </c>
-      <c r="AW8" t="s">
-        <v>197</v>
-      </c>
-      <c r="AX8" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY8" t="s">
-        <v>208</v>
-      </c>
-      <c r="AZ8" t="s">
-        <v>208</v>
-      </c>
-      <c r="BB8" t="s">
-        <v>210</v>
-      </c>
-      <c r="BC8" t="s">
-        <v>210</v>
-      </c>
-      <c r="BD8" t="s">
-        <v>197</v>
-      </c>
-      <c r="BG8" t="s">
-        <v>235</v>
-      </c>
-      <c r="BH8" t="s">
-        <v>197</v>
-      </c>
-      <c r="BI8" t="s">
-        <v>205</v>
-      </c>
-      <c r="BM8" t="s">
-        <v>197</v>
-      </c>
-      <c r="BT8" t="s">
-        <v>198</v>
-      </c>
-      <c r="BU8" t="s">
-        <v>199</v>
-      </c>
-      <c r="BZ8" t="s">
-        <v>212</v>
-      </c>
-      <c r="CC8" t="s">
-        <v>198</v>
-      </c>
-      <c r="CD8" t="s">
-        <v>199</v>
-      </c>
-      <c r="CJ8" t="s">
-        <v>213</v>
-      </c>
-      <c r="CK8" t="s">
-        <v>214</v>
-      </c>
-      <c r="CL8" t="s">
-        <v>215</v>
-      </c>
-      <c r="CP8" t="s">
-        <v>198</v>
-      </c>
-      <c r="CQ8" t="s">
-        <v>199</v>
-      </c>
-      <c r="CU8" t="s">
-        <v>216</v>
-      </c>
-      <c r="CY8" t="s">
-        <v>217</v>
-      </c>
-      <c r="CZ8" t="s">
-        <v>217</v>
-      </c>
-      <c r="DB8" t="s">
-        <v>218</v>
-      </c>
-      <c r="DD8" t="s">
-        <v>213</v>
-      </c>
-      <c r="DE8" t="s">
-        <v>214</v>
-      </c>
-      <c r="DF8" t="s">
-        <v>215</v>
-      </c>
-      <c r="DH8" t="s">
-        <v>219</v>
-      </c>
-      <c r="DJ8" t="s">
-        <v>198</v>
-      </c>
-      <c r="DK8" t="s">
-        <v>199</v>
-      </c>
-      <c r="DO8" t="s">
-        <v>216</v>
-      </c>
-      <c r="DS8" t="s">
-        <v>220</v>
-      </c>
-      <c r="EX8" t="s">
-        <v>213</v>
-      </c>
-      <c r="EY8" t="s">
-        <v>214</v>
-      </c>
-      <c r="EZ8" t="s">
-        <v>215</v>
-      </c>
-      <c r="FB8" t="s">
-        <v>219</v>
-      </c>
-      <c r="FD8" t="s">
-        <v>198</v>
-      </c>
-      <c r="FE8" t="s">
-        <v>199</v>
-      </c>
-      <c r="FI8" t="s">
-        <v>216</v>
-      </c>
-      <c r="FM8" t="s">
-        <v>217</v>
-      </c>
-      <c r="FN8" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:190">
-      <c r="A9">
-        <v>67</v>
-      </c>
-      <c r="B9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D9" t="s">
-        <v>222</v>
-      </c>
-      <c r="E9" t="s">
-        <v>193</v>
-      </c>
-      <c r="M9" t="s">
-        <v>194</v>
-      </c>
-      <c r="O9" t="s">
-        <v>195</v>
-      </c>
-      <c r="P9" t="s">
-        <v>196</v>
-      </c>
-      <c r="R9" t="s">
-        <v>197</v>
-      </c>
-      <c r="S9" t="s">
-        <v>198</v>
-      </c>
-      <c r="T9" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>197</v>
-      </c>
-      <c r="AP9" t="s">
-        <v>234</v>
-      </c>
-      <c r="AQ9" t="s">
-        <v>204</v>
-      </c>
-      <c r="AR9" t="s">
-        <v>205</v>
-      </c>
-      <c r="AS9" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV9" t="s">
-        <v>206</v>
-      </c>
-      <c r="AW9" t="s">
-        <v>197</v>
-      </c>
-      <c r="AX9" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY9" t="s">
-        <v>208</v>
-      </c>
-      <c r="AZ9" t="s">
-        <v>208</v>
-      </c>
-      <c r="BB9" t="s">
-        <v>210</v>
-      </c>
-      <c r="BC9" t="s">
-        <v>210</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>197</v>
-      </c>
-      <c r="BG9" t="s">
-        <v>236</v>
-      </c>
-      <c r="BH9" t="s">
-        <v>197</v>
-      </c>
-      <c r="BI9" t="s">
-        <v>205</v>
-      </c>
-      <c r="BM9" t="s">
-        <v>197</v>
-      </c>
-      <c r="BT9" t="s">
-        <v>198</v>
-      </c>
-      <c r="BU9" t="s">
-        <v>199</v>
-      </c>
-      <c r="BZ9" t="s">
-        <v>212</v>
-      </c>
-      <c r="CC9" t="s">
-        <v>198</v>
-      </c>
-      <c r="CD9" t="s">
-        <v>199</v>
-      </c>
-      <c r="CJ9" t="s">
-        <v>213</v>
-      </c>
-      <c r="CK9" t="s">
-        <v>214</v>
-      </c>
-      <c r="CL9" t="s">
-        <v>215</v>
-      </c>
-      <c r="CP9" t="s">
-        <v>198</v>
-      </c>
-      <c r="CQ9" t="s">
-        <v>199</v>
-      </c>
-      <c r="CU9" t="s">
-        <v>216</v>
-      </c>
-      <c r="CY9" t="s">
-        <v>217</v>
-      </c>
-      <c r="CZ9" t="s">
-        <v>217</v>
-      </c>
-      <c r="DB9" t="s">
-        <v>218</v>
-      </c>
-      <c r="DD9" t="s">
-        <v>213</v>
-      </c>
-      <c r="DE9" t="s">
-        <v>214</v>
-      </c>
-      <c r="DF9" t="s">
-        <v>215</v>
-      </c>
-      <c r="DH9" t="s">
-        <v>219</v>
-      </c>
-      <c r="DJ9" t="s">
-        <v>198</v>
-      </c>
-      <c r="DK9" t="s">
-        <v>199</v>
-      </c>
-      <c r="DO9" t="s">
-        <v>216</v>
-      </c>
-      <c r="DS9" t="s">
-        <v>220</v>
-      </c>
-      <c r="EX9" t="s">
-        <v>213</v>
-      </c>
-      <c r="EY9" t="s">
-        <v>214</v>
-      </c>
-      <c r="EZ9" t="s">
-        <v>215</v>
-      </c>
-      <c r="FB9" t="s">
-        <v>219</v>
-      </c>
-      <c r="FD9" t="s">
-        <v>198</v>
-      </c>
-      <c r="FE9" t="s">
-        <v>199</v>
-      </c>
-      <c r="FI9" t="s">
-        <v>216</v>
-      </c>
-      <c r="FM9" t="s">
-        <v>217</v>
-      </c>
-      <c r="FN9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:190">
-      <c r="A10">
-        <v>68</v>
-      </c>
-      <c r="B10" t="s">
-        <v>233</v>
-      </c>
-      <c r="D10" t="s">
-        <v>222</v>
-      </c>
-      <c r="E10" t="s">
-        <v>193</v>
-      </c>
-      <c r="M10" t="s">
-        <v>194</v>
-      </c>
-      <c r="O10" t="s">
-        <v>195</v>
-      </c>
-      <c r="P10" t="s">
-        <v>196</v>
-      </c>
-      <c r="R10" t="s">
-        <v>197</v>
-      </c>
-      <c r="S10" t="s">
-        <v>198</v>
-      </c>
-      <c r="T10" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>197</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>234</v>
-      </c>
-      <c r="AQ10" t="s">
-        <v>204</v>
-      </c>
-      <c r="AR10" t="s">
-        <v>205</v>
-      </c>
-      <c r="AS10" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV10" t="s">
-        <v>206</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>197</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY10" t="s">
-        <v>208</v>
-      </c>
-      <c r="AZ10" t="s">
-        <v>208</v>
-      </c>
-      <c r="BB10" t="s">
-        <v>210</v>
-      </c>
-      <c r="BC10" t="s">
-        <v>210</v>
-      </c>
-      <c r="BD10" t="s">
-        <v>197</v>
-      </c>
-      <c r="BG10" t="s">
-        <v>237</v>
-      </c>
-      <c r="BH10" t="s">
-        <v>197</v>
-      </c>
-      <c r="BI10" t="s">
-        <v>205</v>
-      </c>
-      <c r="BM10" t="s">
-        <v>197</v>
-      </c>
-      <c r="BT10" t="s">
-        <v>198</v>
-      </c>
-      <c r="BU10" t="s">
-        <v>199</v>
-      </c>
-      <c r="BZ10" t="s">
-        <v>212</v>
-      </c>
-      <c r="CC10" t="s">
-        <v>198</v>
-      </c>
-      <c r="CD10" t="s">
-        <v>199</v>
-      </c>
-      <c r="CJ10" t="s">
-        <v>213</v>
-      </c>
-      <c r="CK10" t="s">
-        <v>214</v>
-      </c>
-      <c r="CL10" t="s">
-        <v>215</v>
-      </c>
-      <c r="CP10" t="s">
-        <v>198</v>
-      </c>
-      <c r="CQ10" t="s">
-        <v>199</v>
-      </c>
-      <c r="CU10" t="s">
-        <v>216</v>
-      </c>
-      <c r="CY10" t="s">
-        <v>217</v>
-      </c>
-      <c r="CZ10" t="s">
-        <v>217</v>
-      </c>
-      <c r="DB10" t="s">
-        <v>218</v>
-      </c>
-      <c r="DD10" t="s">
-        <v>213</v>
-      </c>
-      <c r="DE10" t="s">
-        <v>214</v>
-      </c>
-      <c r="DF10" t="s">
-        <v>215</v>
-      </c>
-      <c r="DH10" t="s">
-        <v>219</v>
-      </c>
-      <c r="DJ10" t="s">
-        <v>198</v>
-      </c>
-      <c r="DK10" t="s">
-        <v>199</v>
-      </c>
-      <c r="DO10" t="s">
-        <v>216</v>
-      </c>
-      <c r="DS10" t="s">
-        <v>220</v>
-      </c>
-      <c r="EX10" t="s">
-        <v>213</v>
-      </c>
-      <c r="EY10" t="s">
-        <v>214</v>
-      </c>
-      <c r="EZ10" t="s">
-        <v>215</v>
-      </c>
-      <c r="FB10" t="s">
-        <v>219</v>
-      </c>
-      <c r="FD10" t="s">
-        <v>198</v>
-      </c>
-      <c r="FE10" t="s">
-        <v>199</v>
-      </c>
-      <c r="FI10" t="s">
-        <v>216</v>
-      </c>
-      <c r="FM10" t="s">
-        <v>217</v>
-      </c>
-      <c r="FN10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:190">
-      <c r="A11">
-        <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>233</v>
-      </c>
-      <c r="D11" t="s">
-        <v>222</v>
-      </c>
-      <c r="E11" t="s">
-        <v>193</v>
-      </c>
-      <c r="M11" t="s">
-        <v>194</v>
-      </c>
-      <c r="O11" t="s">
-        <v>195</v>
-      </c>
-      <c r="P11" t="s">
-        <v>196</v>
-      </c>
-      <c r="R11" t="s">
-        <v>197</v>
-      </c>
-      <c r="S11" t="s">
-        <v>198</v>
-      </c>
-      <c r="T11" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>197</v>
-      </c>
-      <c r="AP11" t="s">
-        <v>234</v>
-      </c>
-      <c r="AQ11" t="s">
-        <v>204</v>
-      </c>
-      <c r="AR11" t="s">
-        <v>205</v>
-      </c>
-      <c r="AS11" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV11" t="s">
-        <v>206</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>197</v>
-      </c>
-      <c r="AX11" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY11" t="s">
-        <v>208</v>
-      </c>
-      <c r="AZ11" t="s">
-        <v>208</v>
-      </c>
-      <c r="BB11" t="s">
-        <v>210</v>
-      </c>
-      <c r="BC11" t="s">
-        <v>210</v>
-      </c>
-      <c r="BD11" t="s">
-        <v>197</v>
-      </c>
-      <c r="BG11" t="s">
-        <v>238</v>
-      </c>
-      <c r="BH11" t="s">
-        <v>197</v>
-      </c>
-      <c r="BI11" t="s">
-        <v>205</v>
-      </c>
-      <c r="BM11" t="s">
-        <v>197</v>
-      </c>
-      <c r="BT11" t="s">
-        <v>198</v>
-      </c>
-      <c r="BU11" t="s">
-        <v>199</v>
-      </c>
-      <c r="BZ11" t="s">
-        <v>212</v>
-      </c>
-      <c r="CC11" t="s">
-        <v>198</v>
-      </c>
-      <c r="CD11" t="s">
-        <v>199</v>
-      </c>
-      <c r="CJ11" t="s">
-        <v>213</v>
-      </c>
-      <c r="CK11" t="s">
-        <v>214</v>
-      </c>
-      <c r="CL11" t="s">
-        <v>215</v>
-      </c>
-      <c r="CP11" t="s">
-        <v>198</v>
-      </c>
-      <c r="CQ11" t="s">
-        <v>199</v>
-      </c>
-      <c r="CU11" t="s">
-        <v>216</v>
-      </c>
-      <c r="CY11" t="s">
-        <v>217</v>
-      </c>
-      <c r="CZ11" t="s">
-        <v>217</v>
-      </c>
-      <c r="DB11" t="s">
-        <v>218</v>
-      </c>
-      <c r="DD11" t="s">
-        <v>213</v>
-      </c>
-      <c r="DE11" t="s">
-        <v>214</v>
-      </c>
-      <c r="DF11" t="s">
-        <v>215</v>
-      </c>
-      <c r="DH11" t="s">
-        <v>219</v>
-      </c>
-      <c r="DJ11" t="s">
-        <v>198</v>
-      </c>
-      <c r="DK11" t="s">
-        <v>199</v>
-      </c>
-      <c r="DO11" t="s">
-        <v>216</v>
-      </c>
-      <c r="DS11" t="s">
-        <v>220</v>
-      </c>
-      <c r="EX11" t="s">
-        <v>213</v>
-      </c>
-      <c r="EY11" t="s">
-        <v>214</v>
-      </c>
-      <c r="EZ11" t="s">
-        <v>215</v>
-      </c>
-      <c r="FB11" t="s">
-        <v>219</v>
-      </c>
-      <c r="FD11" t="s">
-        <v>198</v>
-      </c>
-      <c r="FE11" t="s">
-        <v>199</v>
-      </c>
-      <c r="FI11" t="s">
-        <v>216</v>
-      </c>
-      <c r="FM11" t="s">
-        <v>217</v>
-      </c>
-      <c r="FN11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:190">
-      <c r="A12">
-        <v>70</v>
-      </c>
-      <c r="B12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D12" t="s">
-        <v>222</v>
-      </c>
-      <c r="E12" t="s">
-        <v>193</v>
-      </c>
-      <c r="G12" t="s">
-        <v>228</v>
-      </c>
-      <c r="M12" t="s">
-        <v>194</v>
-      </c>
-      <c r="O12" t="s">
-        <v>195</v>
-      </c>
-      <c r="P12" t="s">
-        <v>196</v>
-      </c>
-      <c r="R12" t="s">
-        <v>197</v>
-      </c>
-      <c r="S12" t="s">
-        <v>198</v>
-      </c>
-      <c r="T12" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>197</v>
-      </c>
-      <c r="AP12" t="s">
-        <v>203</v>
-      </c>
-      <c r="AQ12" t="s">
-        <v>204</v>
-      </c>
-      <c r="AR12" t="s">
-        <v>205</v>
-      </c>
-      <c r="AS12" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU12" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV12" t="s">
-        <v>206</v>
-      </c>
-      <c r="AW12" t="s">
-        <v>197</v>
-      </c>
-      <c r="AX12" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY12" t="s">
-        <v>208</v>
-      </c>
-      <c r="AZ12" t="s">
-        <v>208</v>
-      </c>
-      <c r="BB12" t="s">
-        <v>210</v>
-      </c>
-      <c r="BC12" t="s">
-        <v>210</v>
-      </c>
-      <c r="BD12" t="s">
-        <v>197</v>
-      </c>
-      <c r="BG12" t="s">
-        <v>239</v>
-      </c>
-      <c r="BH12" t="s">
-        <v>197</v>
-      </c>
-      <c r="BI12" t="s">
-        <v>205</v>
-      </c>
-      <c r="BM12" t="s">
-        <v>197</v>
-      </c>
-      <c r="BT12" t="s">
-        <v>198</v>
-      </c>
-      <c r="BU12" t="s">
-        <v>199</v>
-      </c>
-      <c r="BZ12" t="s">
-        <v>212</v>
-      </c>
-      <c r="CC12" t="s">
-        <v>198</v>
-      </c>
-      <c r="CD12" t="s">
-        <v>199</v>
-      </c>
-      <c r="CJ12" t="s">
-        <v>213</v>
-      </c>
-      <c r="CK12" t="s">
-        <v>214</v>
-      </c>
-      <c r="CL12" t="s">
-        <v>215</v>
-      </c>
-      <c r="CP12" t="s">
-        <v>198</v>
-      </c>
-      <c r="CQ12" t="s">
-        <v>199</v>
-      </c>
-      <c r="CU12" t="s">
-        <v>216</v>
-      </c>
-      <c r="CY12" t="s">
-        <v>217</v>
-      </c>
-      <c r="CZ12" t="s">
-        <v>217</v>
-      </c>
-      <c r="DB12" t="s">
-        <v>218</v>
-      </c>
-      <c r="DD12" t="s">
-        <v>213</v>
-      </c>
-      <c r="DE12" t="s">
-        <v>214</v>
-      </c>
-      <c r="DF12" t="s">
-        <v>215</v>
-      </c>
-      <c r="DH12" t="s">
-        <v>219</v>
-      </c>
-      <c r="DJ12" t="s">
-        <v>198</v>
-      </c>
-      <c r="DK12" t="s">
-        <v>199</v>
-      </c>
-      <c r="DO12" t="s">
-        <v>216</v>
-      </c>
-      <c r="DS12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:190">
-      <c r="A13">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s">
-        <v>227</v>
-      </c>
-      <c r="D13" t="s">
-        <v>222</v>
-      </c>
-      <c r="E13" t="s">
-        <v>193</v>
-      </c>
-      <c r="G13" t="s">
-        <v>228</v>
-      </c>
-      <c r="M13" t="s">
-        <v>194</v>
-      </c>
-      <c r="O13" t="s">
-        <v>195</v>
-      </c>
-      <c r="P13" t="s">
-        <v>196</v>
-      </c>
-      <c r="R13" t="s">
-        <v>197</v>
-      </c>
-      <c r="S13" t="s">
-        <v>198</v>
-      </c>
-      <c r="T13" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>197</v>
-      </c>
-      <c r="AP13" t="s">
-        <v>203</v>
-      </c>
-      <c r="AQ13" t="s">
-        <v>204</v>
-      </c>
-      <c r="AR13" t="s">
-        <v>205</v>
-      </c>
-      <c r="AS13" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV13" t="s">
-        <v>206</v>
-      </c>
-      <c r="AW13" t="s">
-        <v>197</v>
-      </c>
-      <c r="AX13" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY13" t="s">
-        <v>208</v>
-      </c>
-      <c r="AZ13" t="s">
-        <v>208</v>
-      </c>
-      <c r="BB13" t="s">
-        <v>210</v>
-      </c>
-      <c r="BC13" t="s">
-        <v>210</v>
-      </c>
-      <c r="BD13" t="s">
-        <v>197</v>
-      </c>
-      <c r="BG13" t="s">
-        <v>240</v>
-      </c>
-      <c r="BH13" t="s">
-        <v>197</v>
-      </c>
-      <c r="BI13" t="s">
-        <v>205</v>
-      </c>
-      <c r="BM13" t="s">
-        <v>197</v>
-      </c>
-      <c r="BT13" t="s">
-        <v>198</v>
-      </c>
-      <c r="BU13" t="s">
-        <v>199</v>
-      </c>
-      <c r="BZ13" t="s">
-        <v>212</v>
-      </c>
-      <c r="CC13" t="s">
-        <v>198</v>
-      </c>
-      <c r="CD13" t="s">
-        <v>199</v>
-      </c>
-      <c r="CJ13" t="s">
-        <v>213</v>
-      </c>
-      <c r="CK13" t="s">
-        <v>214</v>
-      </c>
-      <c r="CL13" t="s">
-        <v>215</v>
-      </c>
-      <c r="CP13" t="s">
-        <v>198</v>
-      </c>
-      <c r="CQ13" t="s">
-        <v>199</v>
-      </c>
-      <c r="CU13" t="s">
-        <v>216</v>
-      </c>
-      <c r="CY13" t="s">
-        <v>217</v>
-      </c>
-      <c r="CZ13" t="s">
-        <v>217</v>
-      </c>
-      <c r="DB13" t="s">
-        <v>218</v>
-      </c>
-      <c r="DD13" t="s">
-        <v>213</v>
-      </c>
-      <c r="DE13" t="s">
-        <v>214</v>
-      </c>
-      <c r="DF13" t="s">
-        <v>215</v>
-      </c>
-      <c r="DH13" t="s">
-        <v>219</v>
-      </c>
-      <c r="DJ13" t="s">
-        <v>198</v>
-      </c>
-      <c r="DK13" t="s">
-        <v>199</v>
-      </c>
-      <c r="DO13" t="s">
-        <v>216</v>
-      </c>
-      <c r="DS13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:190">
-      <c r="A14">
-        <v>72</v>
-      </c>
-      <c r="B14" t="s">
-        <v>227</v>
-      </c>
-      <c r="D14" t="s">
-        <v>222</v>
-      </c>
-      <c r="E14" t="s">
-        <v>193</v>
-      </c>
-      <c r="G14" t="s">
-        <v>228</v>
-      </c>
-      <c r="M14" t="s">
-        <v>194</v>
-      </c>
-      <c r="O14" t="s">
-        <v>195</v>
-      </c>
-      <c r="P14" t="s">
-        <v>196</v>
-      </c>
-      <c r="R14" t="s">
-        <v>197</v>
-      </c>
-      <c r="S14" t="s">
-        <v>198</v>
-      </c>
-      <c r="T14" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>197</v>
-      </c>
-      <c r="AP14" t="s">
-        <v>203</v>
-      </c>
-      <c r="AQ14" t="s">
-        <v>204</v>
-      </c>
-      <c r="AR14" t="s">
-        <v>205</v>
-      </c>
-      <c r="AS14" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV14" t="s">
-        <v>206</v>
-      </c>
-      <c r="AW14" t="s">
-        <v>197</v>
-      </c>
-      <c r="AX14" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY14" t="s">
-        <v>208</v>
-      </c>
-      <c r="AZ14" t="s">
-        <v>208</v>
-      </c>
-      <c r="BB14" t="s">
-        <v>210</v>
-      </c>
-      <c r="BC14" t="s">
-        <v>210</v>
-      </c>
-      <c r="BD14" t="s">
-        <v>197</v>
-      </c>
-      <c r="BG14" t="s">
-        <v>241</v>
-      </c>
-      <c r="BH14" t="s">
-        <v>197</v>
-      </c>
-      <c r="BI14" t="s">
-        <v>205</v>
-      </c>
-      <c r="BM14" t="s">
-        <v>197</v>
-      </c>
-      <c r="BT14" t="s">
-        <v>198</v>
-      </c>
-      <c r="BU14" t="s">
-        <v>199</v>
-      </c>
-      <c r="BZ14" t="s">
-        <v>212</v>
-      </c>
-      <c r="CC14" t="s">
-        <v>198</v>
-      </c>
-      <c r="CD14" t="s">
-        <v>199</v>
-      </c>
-      <c r="CJ14" t="s">
-        <v>213</v>
-      </c>
-      <c r="CK14" t="s">
-        <v>214</v>
-      </c>
-      <c r="CL14" t="s">
-        <v>215</v>
-      </c>
-      <c r="CP14" t="s">
-        <v>198</v>
-      </c>
-      <c r="CQ14" t="s">
-        <v>199</v>
-      </c>
-      <c r="CU14" t="s">
-        <v>216</v>
-      </c>
-      <c r="CY14" t="s">
-        <v>217</v>
-      </c>
-      <c r="CZ14" t="s">
-        <v>217</v>
-      </c>
-      <c r="DB14" t="s">
-        <v>218</v>
-      </c>
-      <c r="DD14" t="s">
-        <v>213</v>
-      </c>
-      <c r="DE14" t="s">
-        <v>214</v>
-      </c>
-      <c r="DF14" t="s">
-        <v>215</v>
-      </c>
-      <c r="DH14" t="s">
-        <v>219</v>
-      </c>
-      <c r="DJ14" t="s">
-        <v>198</v>
-      </c>
-      <c r="DK14" t="s">
-        <v>199</v>
-      </c>
-      <c r="DO14" t="s">
-        <v>216</v>
-      </c>
-      <c r="DS14" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="15" spans="1:190">
-      <c r="A15">
-        <v>74</v>
-      </c>
-      <c r="B15" t="s">
-        <v>227</v>
-      </c>
-      <c r="D15" t="s">
-        <v>222</v>
-      </c>
-      <c r="E15" t="s">
-        <v>193</v>
-      </c>
-      <c r="F15" t="s">
-        <v>242</v>
-      </c>
-      <c r="G15" t="s">
-        <v>243</v>
-      </c>
-      <c r="H15" t="s">
-        <v>244</v>
-      </c>
-      <c r="I15" t="s">
-        <v>242</v>
-      </c>
-      <c r="M15" t="s">
-        <v>194</v>
-      </c>
-      <c r="O15" t="s">
-        <v>195</v>
-      </c>
-      <c r="P15" t="s">
-        <v>196</v>
-      </c>
-      <c r="R15" t="s">
-        <v>197</v>
-      </c>
-      <c r="S15" t="s">
-        <v>198</v>
-      </c>
-      <c r="T15" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>197</v>
-      </c>
-      <c r="AP15" t="s">
-        <v>203</v>
-      </c>
-      <c r="AQ15" t="s">
-        <v>204</v>
-      </c>
-      <c r="AR15" t="s">
-        <v>205</v>
-      </c>
-      <c r="AS15" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU15" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV15" t="s">
-        <v>206</v>
-      </c>
-      <c r="AW15" t="s">
-        <v>197</v>
-      </c>
-      <c r="AX15" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY15" t="s">
-        <v>208</v>
-      </c>
-      <c r="AZ15" t="s">
-        <v>208</v>
-      </c>
-      <c r="BB15" t="s">
-        <v>210</v>
-      </c>
-      <c r="BC15" t="s">
-        <v>210</v>
-      </c>
-      <c r="BD15" t="s">
-        <v>197</v>
-      </c>
-      <c r="BG15" t="s">
-        <v>245</v>
-      </c>
-      <c r="BH15" t="s">
-        <v>197</v>
-      </c>
-      <c r="BI15" t="s">
-        <v>205</v>
-      </c>
-      <c r="BM15" t="s">
-        <v>197</v>
-      </c>
-      <c r="BT15" t="s">
-        <v>198</v>
-      </c>
-      <c r="BU15" t="s">
-        <v>199</v>
-      </c>
-      <c r="BZ15" t="s">
-        <v>212</v>
-      </c>
-      <c r="CC15" t="s">
-        <v>198</v>
-      </c>
-      <c r="CD15" t="s">
-        <v>199</v>
-      </c>
-      <c r="CJ15" t="s">
-        <v>213</v>
-      </c>
-      <c r="CK15" t="s">
-        <v>214</v>
-      </c>
-      <c r="CL15" t="s">
-        <v>215</v>
-      </c>
-      <c r="CP15" t="s">
-        <v>198</v>
-      </c>
-      <c r="CQ15" t="s">
-        <v>199</v>
-      </c>
-      <c r="CU15" t="s">
-        <v>216</v>
-      </c>
-      <c r="CY15" t="s">
-        <v>217</v>
-      </c>
-      <c r="CZ15" t="s">
-        <v>217</v>
-      </c>
-      <c r="DB15" t="s">
-        <v>218</v>
-      </c>
-      <c r="DD15" t="s">
-        <v>213</v>
-      </c>
-      <c r="DE15" t="s">
-        <v>214</v>
-      </c>
-      <c r="DF15" t="s">
-        <v>215</v>
-      </c>
-      <c r="DH15" t="s">
-        <v>219</v>
-      </c>
-      <c r="DJ15" t="s">
-        <v>198</v>
-      </c>
-      <c r="DK15" t="s">
-        <v>199</v>
-      </c>
-      <c r="DO15" t="s">
-        <v>216</v>
-      </c>
-      <c r="DS15" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added download by year,print,sessioStorage
</commit_message>
<xml_diff>
--- a/static/excel/data.xlsx
+++ b/static/excel/data.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="217">
   <si>
     <t>stu_id</t>
   </si>
   <si>
+    <t>stu_image</t>
+  </si>
+  <si>
     <t>stu_name</t>
   </si>
   <si>
@@ -584,6 +587,84 @@
   </si>
   <si>
     <t>pg_cgpa</t>
+  </si>
+  <si>
+    <t>00000basecase.png</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>HINDU</t>
+  </si>
+  <si>
+    <t>ACHARI</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Andaman and Nicobar Islands</t>
+  </si>
+  <si>
+    <t>PhD</t>
+  </si>
+  <si>
+    <t>ACCOUNTS</t>
+  </si>
+  <si>
+    <t>CET</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>2020-21</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>REGULAR</t>
+  </si>
+  <si>
+    <t>00000</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh Board of Intermediate Education</t>
+  </si>
+  <si>
+    <t>1950</t>
+  </si>
+  <si>
+    <t>JANUARY</t>
+  </si>
+  <si>
+    <t>marks</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>puc</t>
+  </si>
+  <si>
+    <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>Science</t>
   </si>
 </sst>
 </file>
@@ -915,13 +996,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:GH1"/>
+  <dimension ref="A1:GI2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:190">
+    <row r="1" spans="1:191">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1491,6 +1572,215 @@
       </c>
       <c r="GH1" t="s">
         <v>189</v>
+      </c>
+      <c r="GI1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:191">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" t="s">
+        <v>193</v>
+      </c>
+      <c r="N2" t="s">
+        <v>194</v>
+      </c>
+      <c r="P2" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>196</v>
+      </c>
+      <c r="S2" t="s">
+        <v>197</v>
+      </c>
+      <c r="T2" t="s">
+        <v>198</v>
+      </c>
+      <c r="U2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>205</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>205</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>206</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>206</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>197</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>207</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>197</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>202</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>197</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>198</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>199</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>208</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>198</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>199</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>209</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>210</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>211</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>198</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>199</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>212</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>214</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>209</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>210</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>211</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>215</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>198</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>199</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>212</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>216</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>209</v>
+      </c>
+      <c r="EZ2" t="s">
+        <v>210</v>
+      </c>
+      <c r="FA2" t="s">
+        <v>211</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>215</v>
+      </c>
+      <c r="FE2" t="s">
+        <v>198</v>
+      </c>
+      <c r="FF2" t="s">
+        <v>199</v>
+      </c>
+      <c r="FJ2" t="s">
+        <v>212</v>
+      </c>
+      <c r="FN2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>209</v>
+      </c>
+      <c r="FS2" t="s">
+        <v>210</v>
+      </c>
+      <c r="FT2" t="s">
+        <v>211</v>
+      </c>
+      <c r="FV2" t="s">
+        <v>215</v>
+      </c>
+      <c r="FX2" t="s">
+        <v>198</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>199</v>
+      </c>
+      <c r="GC2" t="s">
+        <v>212</v>
+      </c>
+      <c r="GG2" t="s">
+        <v>213</v>
+      </c>
+      <c r="GH2" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>